<commit_message>
Connect HDMI Proto output differential lines.
</commit_message>
<xml_diff>
--- a/board/proto-hdmi/skew_calculator.xlsx
+++ b/board/proto-hdmi/skew_calculator.xlsx
@@ -848,10 +848,21 @@
       <c r="G11" s="7">
         <v>200.0</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
+      <c r="H11" s="9">
+        <v>845.44</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" ref="I11:I18" si="2">D11+G11+H11</f>
+        <v>2346.81</v>
+      </c>
+      <c r="J11" s="8">
+        <f>I11-I12</f>
+        <v>-0.55</v>
+      </c>
+      <c r="K11" s="8">
+        <f>MAX(I11:I12)-MAX(I$11:I$18)</f>
+        <v>-0.11</v>
+      </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -877,10 +888,21 @@
       <c r="G12" s="7">
         <v>200.0</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="H12" s="9">
+        <v>1003.45</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="2"/>
+        <v>2347.36</v>
+      </c>
+      <c r="J12" s="8">
+        <f>I12-I11</f>
+        <v>0.55</v>
+      </c>
+      <c r="K12" s="8">
+        <f>MAX(I11:I12)-MAX(I$11:I$18)</f>
+        <v>-0.11</v>
+      </c>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -906,10 +928,21 @@
       <c r="G13" s="7">
         <v>0.0</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="H13" s="9">
+        <v>1078.62</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="2"/>
+        <v>2347.47</v>
+      </c>
+      <c r="J13" s="8">
+        <f>I13-I14</f>
+        <v>0.32</v>
+      </c>
+      <c r="K13" s="8">
+        <f>MAX(I13:I14)-MAX(I$11:I$18)</f>
+        <v>0</v>
+      </c>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -935,10 +968,21 @@
       <c r="G14" s="7">
         <v>0.0</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="H14" s="9">
+        <v>992.67</v>
+      </c>
+      <c r="I14" s="8">
+        <f t="shared" si="2"/>
+        <v>2347.15</v>
+      </c>
+      <c r="J14" s="8">
+        <f>I14-I13</f>
+        <v>-0.32</v>
+      </c>
+      <c r="K14" s="8">
+        <f>MAX(I13:I14)-MAX(I$11:I$18)</f>
+        <v>0</v>
+      </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -964,10 +1008,21 @@
       <c r="G15" s="7">
         <v>200.0</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="H15" s="9">
+        <v>704.88</v>
+      </c>
+      <c r="I15" s="8">
+        <f t="shared" si="2"/>
+        <v>2346.78</v>
+      </c>
+      <c r="J15" s="8">
+        <f>I15-I16</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="8">
+        <f>MAX(I15:I16)-MAX(I$11:I$18)</f>
+        <v>-0.69</v>
+      </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -993,10 +1048,21 @@
       <c r="G16" s="7">
         <v>200.0</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="H16" s="9">
+        <v>672.37</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="2"/>
+        <v>2346.78</v>
+      </c>
+      <c r="J16" s="8">
+        <f>I16-I15</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
+        <f>MAX(I15:I16)-MAX(I$11:I$18)</f>
+        <v>-0.69</v>
+      </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -1022,10 +1088,21 @@
       <c r="G17" s="7">
         <v>0.0</v>
       </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="H17" s="9">
+        <v>797.55</v>
+      </c>
+      <c r="I17" s="8">
+        <f t="shared" si="2"/>
+        <v>2347.47</v>
+      </c>
+      <c r="J17" s="8">
+        <f>I17-I18</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <f>MAX(I17:I18)-MAX(I$11:I$18)</f>
+        <v>0</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1051,10 +1128,21 @@
       <c r="G18" s="7">
         <v>0.0</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="H18" s="9">
+        <v>605.86</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" si="2"/>
+        <v>2347.47</v>
+      </c>
+      <c r="J18" s="8">
+        <f>I18-I17</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
+        <f>MAX(I17:I18)-MAX(I$11:I$18)</f>
+        <v>0</v>
+      </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>

</xml_diff>